<commit_message>
update manifests, date: 2021-02-07, last lines (exp, sim, neg): (16, 12, 10)
</commit_message>
<xml_diff>
--- a/manifests/Experiment_Manifest.xlsx
+++ b/manifests/Experiment_Manifest.xlsx
@@ -913,32 +913,438 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n"/>
-      <c r="F9" s="3" t="n"/>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>e8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>IMG_3174.jpeg</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:50</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0.035976819755617236</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n"/>
-      <c r="F10" s="3" t="n"/>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>e9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IMG_3175.jpeg</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.02565776774681468</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n"/>
-      <c r="F11" s="3" t="n"/>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>e10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>IMG_3176.jpeg</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.0282690393808343</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n"/>
-      <c r="F12" s="3" t="n"/>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>e11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>IMG_3177.jpeg</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.02781007874702744</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n"/>
-      <c r="F13" s="3" t="n"/>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>e12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>IMG_3178.jpeg</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.022924369605732336</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n"/>
-      <c r="F14" s="3" t="n"/>
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>e13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>IMG_3179.jpeg</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.02794206571402925</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n"/>
-      <c r="F15" s="3" t="n"/>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>e14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>IMG_3180.jpeg</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.02224532398965588</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-07, last lines (exp, sim, neg): (23, 17, 14)
</commit_message>
<xml_diff>
--- a/manifests/Experiment_Manifest.xlsx
+++ b/manifests/Experiment_Manifest.xlsx
@@ -1347,32 +1347,438 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n"/>
-      <c r="F16" s="3" t="n"/>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>e15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>IMG_3174.jpeg</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:50</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0.035976819755617236</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n"/>
-      <c r="F17" s="3" t="n"/>
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>e16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>IMG_3175.jpeg</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0.02565776774681468</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n"/>
-      <c r="F18" s="3" t="n"/>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>e17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>IMG_3176.jpeg</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0.0282690393808343</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n"/>
-      <c r="F19" s="3" t="n"/>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>e18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>IMG_3177.jpeg</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0.02781007874702744</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n"/>
-      <c r="F20" s="3" t="n"/>
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>e19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>IMG_3178.jpeg</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0.022924369605732336</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n"/>
-      <c r="F21" s="3" t="n"/>
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>e20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>IMG_3179.jpeg</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0.02794206571402925</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n"/>
-      <c r="F22" s="3" t="n"/>
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>e21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>IMG_3180.jpeg</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>0.02224532398965588</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-07, last lines (exp, sim, neg): (30, 22, 18)
</commit_message>
<xml_diff>
--- a/manifests/Experiment_Manifest.xlsx
+++ b/manifests/Experiment_Manifest.xlsx
@@ -1781,32 +1781,438 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n"/>
-      <c r="F23" s="3" t="n"/>
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>e22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>IMG_3174.jpeg</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:50</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0.035976819755617236</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n"/>
-      <c r="F24" s="3" t="n"/>
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>e23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>IMG_3175.jpeg</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>0.02565776774681468</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n"/>
-      <c r="F25" s="3" t="n"/>
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>e24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>IMG_3176.jpeg</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0.0282690393808343</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n"/>
-      <c r="F26" s="3" t="n"/>
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>e25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>IMG_3177.jpeg</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F26" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>0.02781007874702744</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n"/>
-      <c r="F27" s="3" t="n"/>
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>e26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>IMG_3178.jpeg</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F27" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>0.022924369605732336</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n"/>
-      <c r="F28" s="3" t="n"/>
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>e27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>IMG_3179.jpeg</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F28" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0.02794206571402925</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n"/>
-      <c r="F29" s="3" t="n"/>
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>e28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>IMG_3180.jpeg</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F29" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>0.02224532398965588</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-07, last lines (exp, sim, neg): (9, 7, 6)
</commit_message>
<xml_diff>
--- a/manifests/Experiment_Manifest.xlsx
+++ b/manifests/Experiment_Manifest.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>IMG_3174.jpeg</t>
+          <t>e1_321_1_1.jpeg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>c, s</t>
+          <t>c,s</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -548,7 +548,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>IMG_3175.jpeg</t>
+          <t>e2_321_1_2.jpeg</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -558,7 +558,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>c, s</t>
+          <t>c,s</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IMG_3176.jpeg</t>
+          <t>e3_321_1_3.jpeg</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -620,7 +620,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>c, s</t>
+          <t>c,s</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>IMG_3177.jpeg</t>
+          <t>e4_321_2_2.jpeg</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -682,7 +682,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>c, s</t>
+          <t>c,s</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -734,7 +734,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>IMG_3178.jpeg</t>
+          <t>e5_321_2_1.jpeg</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>c, s</t>
+          <t>c,s</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>IMG_3179.jpeg</t>
+          <t>e6_321_2_0.jpeg</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -806,7 +806,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>c, s</t>
+          <t>c,s</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -858,7 +858,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>IMG_3180.jpeg</t>
+          <t>e7_321_3_1.jpeg</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -868,7 +868,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>c, s</t>
+          <t>c,s</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -913,1306 +913,88 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>e8</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>IMG_3174.jpeg</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A9" s="1" t="n"/>
+      <c r="F9" s="3" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>e9</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>IMG_3175.jpeg</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F10" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A10" s="1" t="n"/>
+      <c r="F10" s="3" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>e10</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>IMG_3176.jpeg</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A11" s="1" t="n"/>
+      <c r="F11" s="3" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>e11</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>IMG_3177.jpeg</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F12" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A12" s="1" t="n"/>
+      <c r="F12" s="3" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>e12</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>IMG_3178.jpeg</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F13" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A13" s="1" t="n"/>
+      <c r="F13" s="3" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>e13</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>IMG_3179.jpeg</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A14" s="1" t="n"/>
+      <c r="F14" s="3" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>e14</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>IMG_3180.jpeg</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A15" s="1" t="n"/>
+      <c r="F15" s="3" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>e15</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>IMG_3174.jpeg</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A16" s="1" t="n"/>
+      <c r="F16" s="3" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>e16</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>IMG_3175.jpeg</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A17" s="1" t="n"/>
+      <c r="F17" s="3" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>e17</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>IMG_3176.jpeg</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F18" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A18" s="1" t="n"/>
+      <c r="F18" s="3" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>e18</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>IMG_3177.jpeg</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F19" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A19" s="1" t="n"/>
+      <c r="F19" s="3" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>e19</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>IMG_3178.jpeg</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F20" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A20" s="1" t="n"/>
+      <c r="F20" s="3" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>e20</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>IMG_3179.jpeg</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F21" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A21" s="1" t="n"/>
+      <c r="F21" s="3" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>e21</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>IMG_3180.jpeg</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F22" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A22" s="1" t="n"/>
+      <c r="F22" s="3" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>e22</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>IMG_3174.jpeg</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F23" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A23" s="1" t="n"/>
+      <c r="F23" s="3" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>e23</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>IMG_3175.jpeg</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F24" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A24" s="1" t="n"/>
+      <c r="F24" s="3" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>e24</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>IMG_3176.jpeg</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F25" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A25" s="1" t="n"/>
+      <c r="F25" s="3" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>e25</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>IMG_3177.jpeg</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F26" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A26" s="1" t="n"/>
+      <c r="F26" s="3" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>e26</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>IMG_3178.jpeg</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F27" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A27" s="1" t="n"/>
+      <c r="F27" s="3" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>e27</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>IMG_3179.jpeg</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F28" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A28" s="1" t="n"/>
+      <c r="F28" s="3" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>e28</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>IMG_3180.jpeg</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F29" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A29" s="1" t="n"/>
+      <c r="F29" s="3" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-07, last lines (exp, sim, neg): (65, 47, 22)
</commit_message>
<xml_diff>
--- a/manifests/Experiment_Manifest.xlsx
+++ b/manifests/Experiment_Manifest.xlsx
@@ -2215,144 +2215,2174 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n"/>
-      <c r="F30" s="3" t="n"/>
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>e29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>e29_321_1_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F30" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:50</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>0.035976819755617236</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n"/>
-      <c r="F31" s="3" t="n"/>
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>e30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>e30_321_1_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F31" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>0.02565776774681468</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n"/>
-      <c r="F32" s="3" t="n"/>
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>e31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>e31_321_1_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F32" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>0.0282690393808343</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n"/>
-      <c r="F33" s="3" t="n"/>
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>e32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>e32_321_2_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F33" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>0.02781007874702744</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n"/>
-      <c r="F34" s="3" t="n"/>
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>e33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>e33_321_2_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F34" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>0.022924369605732336</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n"/>
-      <c r="F35" s="3" t="n"/>
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>e34</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>e34_321_2_0.jpeg</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F35" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>0.02794206571402925</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n"/>
-      <c r="F36" s="3" t="n"/>
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>e35</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>e35_321_3_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F36" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>0.02224532398965588</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n"/>
-      <c r="F37" s="3" t="n"/>
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>e36</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>e36_321_1_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F37" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:50</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>0.035976819755617236</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n"/>
-      <c r="F38" s="3" t="n"/>
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>e37</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>e37_321_1_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F38" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>0.02565776774681468</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n"/>
-      <c r="F39" s="3" t="n"/>
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>e38</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>e38_321_1_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F39" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>0.0282690393808343</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n"/>
-      <c r="F40" s="3" t="n"/>
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>e39</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>e39_321_2_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>0.02781007874702744</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n"/>
-      <c r="F41" s="3" t="n"/>
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>e40</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>e40_321_2_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>0.022924369605732336</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n"/>
-      <c r="F42" s="3" t="n"/>
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>e41</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>e41_321_2_0.jpeg</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>0.02794206571402925</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n"/>
-      <c r="F43" s="3" t="n"/>
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>e42</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>e42_321_3_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>0.02224532398965588</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n"/>
-      <c r="F44" s="3" t="n"/>
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>e43</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>e43_321_1_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:50</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>0.035976819755617236</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n"/>
-      <c r="F45" s="3" t="n"/>
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>e44</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>e44_321_1_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F45" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>0.02565776774681468</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n"/>
-      <c r="F46" s="3" t="n"/>
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>e45</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>e45_321_1_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>0.0282690393808343</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n"/>
-      <c r="F47" s="3" t="n"/>
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>e46</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>e46_321_2_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>0.02781007874702744</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n"/>
-      <c r="F48" s="3" t="n"/>
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>e47</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>e47_321_2_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F48" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>0.022924369605732336</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n"/>
-      <c r="F49" s="3" t="n"/>
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>e48</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>e48_321_2_0.jpeg</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F49" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>0.02794206571402925</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n"/>
-      <c r="F50" s="3" t="n"/>
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>e49</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>e49_321_3_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F50" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>0.02224532398965588</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n"/>
-      <c r="F51" s="3" t="n"/>
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>e50</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>e50_321_1_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F51" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:50</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>0.035976819755617236</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n"/>
-      <c r="F52" s="3" t="n"/>
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>e51</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>e51_321_1_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F52" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>0.02565776774681468</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n"/>
-      <c r="F53" s="3" t="n"/>
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>e52</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>e52_321_1_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F53" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>0.0282690393808343</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n"/>
-      <c r="F54" s="3" t="n"/>
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>e53</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>e53_321_2_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F54" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>0.02781007874702744</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n"/>
-      <c r="F55" s="3" t="n"/>
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>e54</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>e54_321_2_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F55" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>0.022924369605732336</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n"/>
-      <c r="F56" s="3" t="n"/>
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>e55</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>e55_321_2_0.jpeg</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F56" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>0.02794206571402925</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n"/>
-      <c r="F57" s="3" t="n"/>
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>e56</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>e56_321_3_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F57" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>0.02224532398965588</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n"/>
-      <c r="F58" s="3" t="n"/>
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>e57</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>e57_321_1_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F58" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:50</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>0.035976819755617236</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n"/>
-      <c r="F59" s="3" t="n"/>
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>e58</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>e58_321_1_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F59" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>0.02565776774681468</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n"/>
-      <c r="F60" s="3" t="n"/>
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>e59</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>e59_321_1_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F60" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>0.0282690393808343</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n"/>
-      <c r="F61" s="3" t="n"/>
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>e60</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>e60_321_2_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F61" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>0.02781007874702744</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n"/>
-      <c r="F62" s="3" t="n"/>
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>e61</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>e61_321_2_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F62" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>0.022924369605732336</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n"/>
-      <c r="F63" s="3" t="n"/>
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>e62</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>e62_321_2_0.jpeg</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F63" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>0.02794206571402925</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="n"/>
-      <c r="F64" s="3" t="n"/>
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>e63</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>e63_321_3_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F64" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>0.02224532398965588</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-07, last lines (exp, sim, neg): (72, 52, 26)
</commit_message>
<xml_diff>
--- a/manifests/Experiment_Manifest.xlsx
+++ b/manifests/Experiment_Manifest.xlsx
@@ -4385,32 +4385,438 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="n"/>
-      <c r="F65" s="3" t="n"/>
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>e64</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>e64_321_1_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F65" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:50</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>0.035976819755617236</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="n"/>
-      <c r="F66" s="3" t="n"/>
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>e65</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>e65_321_1_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F66" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>0.02565776774681468</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n"/>
-      <c r="F67" s="3" t="n"/>
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>e66</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>e66_321_1_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F67" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>0.0282690393808343</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="n"/>
-      <c r="F68" s="3" t="n"/>
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>e67</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>e67_321_2_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F68" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>0.02781007874702744</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="n"/>
-      <c r="F69" s="3" t="n"/>
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>e68</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>e68_321_2_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F69" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>0.022924369605732336</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="n"/>
-      <c r="F70" s="3" t="n"/>
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>e69</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>e69_321_2_0.jpeg</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F70" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>0.02794206571402925</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="n"/>
-      <c r="F71" s="3" t="n"/>
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>e70</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>e70_321_3_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>wn</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>c,s</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="F71" s="3" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>0.02224532398965588</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n"/>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-11, last lines (exp, sim, neg): (30, 70, 30)
</commit_message>
<xml_diff>
--- a/manifests/Experiment_Manifest.xlsx
+++ b/manifests/Experiment_Manifest.xlsx
@@ -396,10 +396,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10001"/>
+  <dimension ref="A1:M10001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
-      <selection activeCell="L57" sqref="A2:L57"/>
+      <selection activeCell="M29" sqref="A2:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -411,9 +411,11 @@
     <col width="10.26953125" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
     <col width="17.81640625" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
     <col width="37" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
-    <col width="15.90625" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
+    <col width="19.08984375" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
     <col width="18.90625" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
-    <col width="19.36328125" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
+    <col width="122" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
+    <col width="18.6328125" bestFit="1" customWidth="1" style="2" min="12" max="12"/>
+    <col width="21.6328125" bestFit="1" customWidth="1" style="2" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -429,50 +431,55 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>#original_file_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>#warehouse</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>#location</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>#granite_type</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>#slab_id</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>#date_time</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>#latitude_longitude</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>#grain_density</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>#grain_stats(mm)(number_of_grains, mean_grain_size, median_grain_size, grain_size_25_percentile, grain_size_75_percentile)</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>#glare_area(mm^2)</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>#number_of_columns</t>
         </is>
@@ -486,57 +493,62 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>e1_321_1_1.jpeg</t>
+          <t>e1_24019-32_1_1.jpeg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3174.jpeg</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>2020-07-09 15:28:50</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>0.035976819755617236</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -548,57 +560,58 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>e2_321_1_2.jpeg</t>
+          <t>e2_24019-32_1_2.jpeg</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3174HorFlip.jpeg</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+          <t>0.03601408398841037</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>(557, 1.2034423034908583, 0.622372159090909, 0.3788352272727272, 1.2151003117776003)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -610,57 +623,58 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>e3_321_1_3.jpeg</t>
+          <t>e3_24019-32_1_3.jpeg</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3174HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+          <t>0.03598514273146951</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
+          <t>(556, 1.2118453452616824, 0.620386921669759, 0.3788352272727272, 1.2362805279500524)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -672,57 +686,58 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>e4_321_2_2.jpeg</t>
+          <t>e4_24019-32_1_4.jpeg</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3174VertFlip.jpeg</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+          <t>0.03597970442338422</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
+          <t>(556, 1.2112043644478063, 0.622372159090909, 0.3788352272727272, 1.2265241846063397)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -734,57 +749,62 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>e5_321_2_1.jpeg</t>
+          <t>e5_24019-32_1_5.jpeg</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3175.jpeg</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:35</t>
+          <t>24019-32</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+          <t>0.02565776774681468</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -796,57 +816,58 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>e6_321_2_0.jpeg</t>
+          <t>e6_24019-32_1_6.jpeg</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3175HorFlip.jpeg</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+          <t>0.025394039646036728</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
+          <t>(426, 1.2006815483660267, 0.6640522875816992, 0.44270152505446614, 1.313706941723645)</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -858,57 +879,58 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>e7_321_3_1.jpeg</t>
+          <t>e7_24019-32_1_7.jpeg</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3175HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+          <t>0.025684071336918517</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
+          <t>(426, 1.1983660129070648, 0.658482735849933, 0.4169990440320076, 1.345944428094168)</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -920,57 +942,58 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>e8_321_1_1.jpeg</t>
+          <t>e8_24019-32_1_8.jpeg</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3175VertFlip.jpeg</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+          <t>0.025661179302674014</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
+          <t>(429, 1.194463632387686, 0.6640522875816992, 0.415032679738562, 1.3180346695693466)</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -982,57 +1005,62 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>e9_321_1_2.jpeg</t>
+          <t>e9_24019-32_2_7.jpeg</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3176.jpeg</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2020-07-09 15:28:55</t>
+          <t>24019-32</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+          <t>0.0282690393808343</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1044,57 +1072,58 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>e10_321_1_3.jpeg</t>
+          <t>e10_24019-32_2_6.jpeg</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3176HorFlip.jpeg</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+          <t>0.02837290052011066</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
+          <t>(406, 1.3062528016550026, 0.7194086263964772, 0.44166235732935555, 1.3709102149771604)</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1106,57 +1135,58 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>e11_321_2_2.jpeg</t>
+          <t>e11_24019-32_2_5.jpeg</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3176HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+          <t>0.028284673873777706</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
+          <t>(411, 1.2941792768850942, 0.7210545726884368, 0.45292170789506925, 1.3747710729450187)</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1168,57 +1198,58 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>e12_321_2_1.jpeg</t>
+          <t>e12_24019-32_2_4.jpeg</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3176VertFlip.jpeg</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+          <t>0.02827875681952528</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
+          <t>(411, 1.2936517189204129, 0.7141164074561062, 0.449920644955938, 1.373645483931949)</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1230,57 +1261,62 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>e13_321_2_0.jpeg</t>
+          <t>e13_24019-32_2_3.jpeg</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3177.jpeg</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:46</t>
+          <t>24019-32</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+          <t>0.02781007874702744</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1292,57 +1328,58 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>e14_321_3_1.jpeg</t>
+          <t>e14_24019-32_2_2.jpeg</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3177HorFlip.jpeg</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+          <t>0.027876102900504404</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
+          <t>(431, 1.2052792202714877, 0.6884712685218648, 0.44062161185399346, 1.2898082797822203)</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1354,57 +1391,58 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>e15_321_1_1.jpeg</t>
+          <t>e15_24019-32_2_1.jpeg</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3177HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+          <t>0.02787649473524314</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
+          <t>(422, 1.228568973655914, 0.6907582591933163, 0.44062161185399346, 1.321336896284785)</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1416,57 +1454,58 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>e16_321_1_2.jpeg</t>
+          <t>e16_24019-32_2_0.jpeg</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3177VertFlip.jpeg</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+          <t>0.027881343690134994</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
+          <t>(425, 1.2178382287955398, 0.6815190521645917, 0.44062161185399346, 1.2912806737959508)</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1478,57 +1517,62 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>e17_321_1_3.jpeg</t>
+          <t>e17_24019-32_3_1.jpeg</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3178.jpeg</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:05</t>
+          <t>24019-32</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+          <t>0.022924369605732336</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1540,57 +1584,58 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>e18_321_2_2.jpeg</t>
+          <t>e18_24019-32_3_2.jpeg</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3178HorFlip.jpeg</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+          <t>0.022951144256081208</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
+          <t>(460, 1.17172470237719, 0.6598344953300344, 0.4327906096175691, 1.2442618019573477)</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1602,57 +1647,58 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>e19_321_2_1.jpeg</t>
+          <t>e19_24019-32_3_3.jpeg</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3178HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+          <t>0.02298512333041954</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
+          <t>(466, 1.1607730163946821, 0.6347595607724347, 0.4044505270034219, 1.2392886214067258)</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1664,57 +1710,58 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>e20_321_2_0.jpeg</t>
+          <t>e20_24019-32_3_4.jpeg</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3178VertFlip.jpeg</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+          <t>0.02291517590049206</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
+          <t>(462, 1.1679289713086738, 0.6399628547623702, 0.461643316925407, 1.246042901247536)</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1726,57 +1773,62 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>e21_321_3_1.jpeg</t>
+          <t>e21_24019-32_3_5.jpeg</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3179.jpeg</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:53</t>
+          <t>24019-32</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+          <t>0.02794206571402925</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1788,57 +1840,58 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>e22_321_1_1.jpeg</t>
+          <t>e22_24019-32_3_6.jpeg</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3179HorFlip.jpeg</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+          <t>0.027880598655863054</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
+          <t>(434, 1.261013295913934, 0.6870335786355479, 0.42138551292729076, 1.3927012515556347)</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1850,57 +1903,58 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>e23_321_1_2.jpeg</t>
+          <t>e23_24019-32_3_7.jpeg</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3179HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+          <t>0.027892838384476062</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
+          <t>(438, 1.255288969731367, 0.67023202554863, 0.4169702716525152, 1.390751649841509)</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1912,57 +1966,58 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>e24_321_1_3.jpeg</t>
+          <t>e24_24019-32_3_8.jpeg</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3179VertFlip.jpeg</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+          <t>0.027949688702902264</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
+          <t>(439, 1.2525909080286008, 0.7106554032611887, 0.45301985167819075, 1.3746879895680673)</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1974,57 +2029,62 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>e25_321_2_2.jpeg</t>
+          <t>e25_24019-32_4_7.jpeg</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3180.jpeg</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:29</t>
+          <t>24019-32</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+          <t>0.02224532398965588</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -2036,57 +2096,58 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>e26_321_2_1.jpeg</t>
+          <t>e26_24019-32_4_6.jpeg</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3180HorFlip.jpeg</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+          <t>0.022329138304936463</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
+          <t>(405, 1.2056513581677402, 0.6295155839279007, 0.4578295155839278, 1.2412141443786293)</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -2098,57 +2159,58 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>e27_321_2_0.jpeg</t>
+          <t>e27_24019-32_4_5.jpeg</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3180HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+          <t>0.022353515843954976</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
+          <t>(404, 1.2076887508330563, 0.6295155839279007, 0.4578295155839278, 1.238556539327241)</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -2160,2663 +2222,228 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>e28_321_3_1.jpeg</t>
+          <t>e28_24019-32_4_4.jpeg</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>wn</t>
+          <t>IMG_3180VertFlip.jpeg</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>c,s</t>
+          <t>United Stone International</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Solon, Ohio</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Dallas White</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
         <is>
           <t>None, None</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+          <t>0.022329032545548095</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
+          <t>(399, 1.2079370810407037, 0.6295155839279007, 0.4578295155839278, 1.208907754935909)</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>e29</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>e29_321_1_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F30" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A30" s="1" t="n"/>
+      <c r="F30" s="3" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>e30</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>e30_321_1_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F31" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A31" s="1" t="n"/>
+      <c r="F31" s="3" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>e31</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>e31_321_1_3.jpeg</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F32" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A32" s="1" t="n"/>
+      <c r="F32" s="3" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>e32</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>e32_321_2_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F33" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A33" s="1" t="n"/>
+      <c r="F33" s="3" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>e33</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>e33_321_2_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F34" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A34" s="1" t="n"/>
+      <c r="F34" s="3" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>e34</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>e34_321_2_0.jpeg</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F35" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A35" s="1" t="n"/>
+      <c r="F35" s="3" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>e35</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>e35_321_3_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F36" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A36" s="1" t="n"/>
+      <c r="F36" s="3" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>e36</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>e36_321_1_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F37" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A37" s="1" t="n"/>
+      <c r="F37" s="3" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>e37</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>e37_321_1_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F38" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A38" s="1" t="n"/>
+      <c r="F38" s="3" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>e38</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>e38_321_1_3.jpeg</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F39" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A39" s="1" t="n"/>
+      <c r="F39" s="3" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>e39</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>e39_321_2_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F40" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A40" s="1" t="n"/>
+      <c r="F40" s="3" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
-        <is>
-          <t>e40</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>e40_321_2_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F41" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A41" s="1" t="n"/>
+      <c r="F41" s="3" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>e41</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>e41_321_2_0.jpeg</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F42" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A42" s="1" t="n"/>
+      <c r="F42" s="3" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>e42</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>e42_321_3_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F43" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A43" s="1" t="n"/>
+      <c r="F43" s="3" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>e43</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>e43_321_1_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F44" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A44" s="1" t="n"/>
+      <c r="F44" s="3" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>e44</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>e44_321_1_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F45" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A45" s="1" t="n"/>
+      <c r="F45" s="3" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>e45</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>e45_321_1_3.jpeg</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F46" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A46" s="1" t="n"/>
+      <c r="F46" s="3" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>e46</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>e46_321_2_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F47" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A47" s="1" t="n"/>
+      <c r="F47" s="3" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>e47</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>e47_321_2_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F48" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A48" s="1" t="n"/>
+      <c r="F48" s="3" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>e48</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>e48_321_2_0.jpeg</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F49" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A49" s="1" t="n"/>
+      <c r="F49" s="3" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>e49</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>e49_321_3_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F50" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A50" s="1" t="n"/>
+      <c r="F50" s="3" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>e50</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>e50_321_1_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F51" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A51" s="1" t="n"/>
+      <c r="F51" s="3" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>e51</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>e51_321_1_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F52" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A52" s="1" t="n"/>
+      <c r="F52" s="3" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="inlineStr">
-        <is>
-          <t>e52</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>e52_321_1_3.jpeg</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F53" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A53" s="1" t="n"/>
+      <c r="F53" s="3" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>e53</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>e53_321_2_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F54" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A54" s="1" t="n"/>
+      <c r="F54" s="3" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>e54</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>e54_321_2_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F55" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A55" s="1" t="n"/>
+      <c r="F55" s="3" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>e55</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>e55_321_2_0.jpeg</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F56" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A56" s="1" t="n"/>
+      <c r="F56" s="3" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>e56</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>e56_321_3_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F57" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A57" s="1" t="n"/>
+      <c r="F57" s="3" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>e57</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>e57_321_1_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F58" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A58" s="1" t="n"/>
+      <c r="F58" s="3" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>e58</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>e58_321_1_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F59" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A59" s="1" t="n"/>
+      <c r="F59" s="3" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>e59</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>e59_321_1_3.jpeg</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F60" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A60" s="1" t="n"/>
+      <c r="F60" s="3" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>e60</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>e60_321_2_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F61" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A61" s="1" t="n"/>
+      <c r="F61" s="3" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>e61</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>e61_321_2_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F62" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A62" s="1" t="n"/>
+      <c r="F62" s="3" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>e62</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>e62_321_2_0.jpeg</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F63" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A63" s="1" t="n"/>
+      <c r="F63" s="3" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>e63</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>e63_321_3_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F64" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A64" s="1" t="n"/>
+      <c r="F64" s="3" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>e64</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>e64_321_1_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F65" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:50</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>0.035976819755617236</t>
-        </is>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A65" s="1" t="n"/>
+      <c r="F65" s="3" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>e65</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>e65_321_1_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F66" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:28:55</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>0.02565776774681468</t>
-        </is>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A66" s="1" t="n"/>
+      <c r="F66" s="3" t="n"/>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>e66</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>e66_321_1_3.jpeg</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F67" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:05</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>0.0282690393808343</t>
-        </is>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A67" s="1" t="n"/>
+      <c r="F67" s="3" t="n"/>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>e67</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>e67_321_2_2.jpeg</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F68" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:29</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>0.02781007874702744</t>
-        </is>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A68" s="1" t="n"/>
+      <c r="F68" s="3" t="n"/>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>e68</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>e68_321_2_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F69" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:35</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>0.022924369605732336</t>
-        </is>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A69" s="1" t="n"/>
+      <c r="F69" s="3" t="n"/>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>e69</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>e69_321_2_0.jpeg</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F70" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:46</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>0.02794206571402925</t>
-        </is>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
-        </is>
-      </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A70" s="1" t="n"/>
+      <c r="F70" s="3" t="n"/>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="inlineStr">
-        <is>
-          <t>e70</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>e70_321_3_1.jpeg</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>wn</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>c,s</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>gt</t>
-        </is>
-      </c>
-      <c r="F71" s="3" t="inlineStr">
-        <is>
-          <t>321</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>2020-07-09 15:29:53</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>None, None</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>0.02224532398965588</t>
-        </is>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A71" s="1" t="n"/>
+      <c r="F71" s="3" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n"/>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-12, last lines (exp, sim, neg): (64, 104, 26)
</commit_message>
<xml_diff>
--- a/manifests/Experiment_Manifest.xlsx
+++ b/manifests/Experiment_Manifest.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:M10001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
-      <selection activeCell="M29" sqref="A2:M29"/>
+      <selection activeCell="A30" sqref="A30:M93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -588,7 +588,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -651,7 +650,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -714,7 +712,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -844,7 +841,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -907,7 +903,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -970,7 +965,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1100,7 +1094,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1163,7 +1156,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1226,7 +1218,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1356,7 +1347,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1419,7 +1409,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1482,7 +1471,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1612,7 +1600,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1675,7 +1662,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1738,7 +1724,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1868,7 +1853,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1931,7 +1915,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1994,7 +1977,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2124,7 +2106,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2187,7 +2168,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2250,7 +2230,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2278,477 +2257,2608 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n"/>
-      <c r="F30" s="3" t="n"/>
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>e29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>e29_24019-32_1_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>IMG_3070 - Copy.jpeg</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F30" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:33:40</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>0.10626314137255605</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>(1766, 1.2229455581121895, 0.6614104882459312, 0.413381555153707, 1.2921876388374214)</t>
+        </is>
+      </c>
+      <c r="L30" s="1" t="inlineStr">
+        <is>
+          <t>165.27474785372564</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n"/>
-      <c r="F31" s="3" t="n"/>
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>e30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>e30_24019-32_1_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>IMG_3070.jpeg</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F31" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:33:40</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>0.10626314137255605</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>(1766, 1.2229455581121895, 0.6614104882459312, 0.413381555153707, 1.2921876388374214)</t>
+        </is>
+      </c>
+      <c r="L31" s="1" t="inlineStr">
+        <is>
+          <t>165.27474785372564</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n"/>
-      <c r="F32" s="3" t="n"/>
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>e31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>e31_24019-32_1_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>IMG_3070HorFlip - Copy.jpeg</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F32" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>0.10629850658417507</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>(1766, 1.2199003546381992, 0.6614104882459312, 0.413381555153707, 1.2678898364915758)</t>
+        </is>
+      </c>
+      <c r="L32" s="1" t="inlineStr">
+        <is>
+          <t>176.2933681716365</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n"/>
-      <c r="F33" s="3" t="n"/>
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>e32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>e32_24019-32_1_4.jpeg</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>IMG_3070HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F33" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>0.10629850658417507</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>(1766, 1.2199003546381992, 0.6614104882459312, 0.413381555153707, 1.2678898364915758)</t>
+        </is>
+      </c>
+      <c r="L33" s="1" t="inlineStr">
+        <is>
+          <t>176.2933681716365</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n"/>
-      <c r="F34" s="3" t="n"/>
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>e33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>e33_24019-32_1_5.jpeg</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>IMG_3070HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F34" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>0.10635143177604318</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>(1762, 1.225678035511058, 0.6614104882459312, 0.413381555153707, 1.2904231659976855)</t>
+        </is>
+      </c>
+      <c r="L34" s="1" t="inlineStr">
+        <is>
+          <t>171.15013017929488</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n"/>
-      <c r="F35" s="3" t="n"/>
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>e34</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>e34_24019-32_1_6.jpeg</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>IMG_3070VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F35" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>0.10632121683796092</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>(1765, 1.2229526718381063, 0.6614104882459312, 0.413381555153707, 1.2822941522156464)</t>
+        </is>
+      </c>
+      <c r="L35" s="1" t="inlineStr">
+        <is>
+          <t>172.45188887966015</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n"/>
-      <c r="F36" s="3" t="n"/>
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>e35</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>e35_24019-32_1_7.jpeg</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>IMG_3071.jpeg</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F36" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:33:48</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>0.08643496713420627</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>(1684, 1.2069945549279888, 0.708973149761974, 0.4385611510791366, 1.3806035251687194)</t>
+        </is>
+      </c>
+      <c r="L36" s="1" t="inlineStr">
+        <is>
+          <t>94.42038980384035</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n"/>
-      <c r="F37" s="3" t="n"/>
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>e36</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>e36_24019-32_1_8.jpeg</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>IMG_3071HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F37" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>0.08652764479064227</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>(1694, 1.2008022668874019, 0.6863044771772961, 0.4385611510791366, 1.3775864387972148)</t>
+        </is>
+      </c>
+      <c r="L37" s="1" t="inlineStr">
+        <is>
+          <t>100.28212637027066</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n"/>
-      <c r="F38" s="3" t="n"/>
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>e37</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>e37_24019-32_2_7.jpeg</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>IMG_3071HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F38" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>0.08649615379638731</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>(1690, 1.2043601987317867, 0.6989554419433464, 0.4385611510791366, 1.3803898557031795)</t>
+        </is>
+      </c>
+      <c r="L38" s="1" t="inlineStr">
+        <is>
+          <t>98.4263856218622</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n"/>
-      <c r="F39" s="3" t="n"/>
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>e38</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>e38_24019-32_2_6.jpeg</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>IMG_3071VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F39" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>0.08645835489881472</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>(1696, 1.199935426463319, 0.6956412016185844, 0.4385611510791366, 1.366295785404334)</t>
+        </is>
+      </c>
+      <c r="L39" s="1" t="inlineStr">
+        <is>
+          <t>98.1003161948139</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n"/>
-      <c r="F40" s="3" t="n"/>
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>e39</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>e39_24019-32_2_5.jpeg</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>IMG_3072.jpeg</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:33:56</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>0.13068273945587136</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>(1502, 1.3665101504291362, 0.6695283064779868, 0.4430232558139534, 1.358199999090961)</t>
+        </is>
+      </c>
+      <c r="L40" s="1" t="inlineStr">
+        <is>
+          <t>143.29521206564354</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n"/>
-      <c r="F41" s="3" t="n"/>
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>e40</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>e40_24019-32_2_4.jpeg</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>IMG_3072HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>0.13067947148374115</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>(1496, 1.3698571109802948, 0.6695283064779868, 0.4430232558139534, 1.3584396791263003)</t>
+        </is>
+      </c>
+      <c r="L41" s="1" t="inlineStr">
+        <is>
+          <t>145.40357696516693</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n"/>
-      <c r="F42" s="3" t="n"/>
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>e41</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>e41_24019-32_2_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>IMG_3072HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>0.13067630254106943</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>(1494, 1.3735578691894301, 0.6767066767292842, 0.4430232558139534, 1.3801462356689742)</t>
+        </is>
+      </c>
+      <c r="L42" s="1" t="inlineStr">
+        <is>
+          <t>145.38977675855187</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n"/>
-      <c r="F43" s="3" t="n"/>
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>e42</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>e42_24019-32_2_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>IMG_3072VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>0.1306894239443195</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>(1496, 1.3723766916619047, 0.6735267681936303, 0.4430232558139534, 1.3741309807445359)</t>
+        </is>
+      </c>
+      <c r="L43" s="1" t="inlineStr">
+        <is>
+          <t>145.88505084040355</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n"/>
-      <c r="F44" s="3" t="n"/>
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>e43</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>e43_24019-32_2_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>IMG_3073.jpeg</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:34:06</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>0.10439114517834187</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>(1211, 1.5302384468465018, 0.8603792236850193, 0.5311338289962824, 1.7103870535757584)</t>
+        </is>
+      </c>
+      <c r="L44" s="1" t="inlineStr">
+        <is>
+          <t>5.845177149984105</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n"/>
-      <c r="F45" s="3" t="n"/>
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>e44</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>e44_24019-32_2_0.jpeg</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>IMG_3073HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F45" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>0.104415518416343</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>(1214, 1.529431913959941, 0.8610819429311831, 0.5311338289962824, 1.7238646636287058)</t>
+        </is>
+      </c>
+      <c r="L45" s="1" t="inlineStr">
+        <is>
+          <t>5.988109409764926</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n"/>
-      <c r="F46" s="3" t="n"/>
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>e45</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>e45_24019-32_3_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>IMG_3073HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>0.10442685480611097</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>(1218, 1.5254308696049177, 0.8315038816623117, 0.5311338289962824, 1.709941190842706)</t>
+        </is>
+      </c>
+      <c r="L46" s="1" t="inlineStr">
+        <is>
+          <t>6.253913261287154</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n"/>
-      <c r="F47" s="3" t="n"/>
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>e46</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>e46_24019-32_3_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>IMG_3073VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>0.10446936626774085</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>(1218, 1.525646741059214, 0.8514802573194831, 0.5311338289962824, 1.7173242797459052)</t>
+        </is>
+      </c>
+      <c r="L47" s="1" t="inlineStr">
+        <is>
+          <t>6.268958762316714</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n"/>
-      <c r="F48" s="3" t="n"/>
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>e47</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>e47_24019-32_3_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>IMG_3074.jpeg</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F48" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:34:22</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>0.11056792245481</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>(1088, 1.676076645824256, 0.913030454318522, 0.5885471491007104, 1.8759228734454052)</t>
+        </is>
+      </c>
+      <c r="L48" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n"/>
-      <c r="F49" s="3" t="n"/>
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>e48</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>e48_24019-32_3_4.jpeg</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>IMG_3074HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F49" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>0.11065494244903235</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>(1091, 1.6715908328300884, 0.913030454318522, 0.6014683101867633, 1.8816739199934616)</t>
+        </is>
+      </c>
+      <c r="L49" s="1" t="inlineStr">
+        <is>
+          <t>3.143459468809765</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n"/>
-      <c r="F50" s="3" t="n"/>
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>e49</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>e49_24019-32_3_5.jpeg</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>IMG_3074HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F50" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>0.11066092448945149</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>(1087, 1.678747266795845, 0.913030454318522, 0.5813002364269473, 1.8866639498871733)</t>
+        </is>
+      </c>
+      <c r="L50" s="1" t="inlineStr">
+        <is>
+          <t>4.914911766150074</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n"/>
-      <c r="F51" s="3" t="n"/>
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>e50</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>e50_24019-32_3_6.jpeg</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>IMG_3074VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F51" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>0.11057754980110956</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>(1081, 1.68491820145904, 0.913030454318522, 0.5946935894189962, 1.9057548714019261)</t>
+        </is>
+      </c>
+      <c r="L51" s="1" t="inlineStr">
+        <is>
+          <t>3.1203032296288455</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n"/>
-      <c r="F52" s="3" t="n"/>
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>e51</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>e51_24019-32_3_7.jpeg</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>IMG_3075.jpeg</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F52" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:34:29</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>0.08209072082885052</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>(1118, 1.4621469360083703, 0.9200331451356919, 0.608079800498753, 1.7115512495008964)</t>
+        </is>
+      </c>
+      <c r="L52" s="1" t="inlineStr">
+        <is>
+          <t>6.860800616911583</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n"/>
-      <c r="F53" s="3" t="n"/>
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>e52</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>e52_24019-32_3_8.jpeg</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>IMG_3075HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F53" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>0.08200434076902503</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>(1126, 1.4496896359848837, 0.903816929338094, 0.572775744271396, 1.6973093081113473)</t>
+        </is>
+      </c>
+      <c r="L53" s="1" t="inlineStr">
+        <is>
+          <t>9.08514439586818</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n"/>
-      <c r="F54" s="3" t="n"/>
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>e53</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>e53_24019-32_4_7.jpeg</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>IMG_3075HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F54" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>0.0820862432447559</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>(1121, 1.4589576859822246, 0.917424833211809, 0.6008683417975496, 1.6987361241863967)</t>
+        </is>
+      </c>
+      <c r="L54" s="1" t="inlineStr">
+        <is>
+          <t>7.767870677421157</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n"/>
-      <c r="F55" s="3" t="n"/>
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>e54</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>e54_24019-32_4_6.jpeg</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>IMG_3075VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F55" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>0.08209650437497275</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>(1117, 1.4629038457113364, 0.9376825215863195, 0.608079800498753, 1.7104042501193422)</t>
+        </is>
+      </c>
+      <c r="L55" s="1" t="inlineStr">
+        <is>
+          <t>6.387044279575373</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n"/>
-      <c r="F56" s="3" t="n"/>
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>e55</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>e55_24019-32_4_5.jpeg</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>IMG_3076.jpeg</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F56" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:34:40</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>0.13693333894453324</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>(909, 2.084359830935198, 1.2117431192660548, 0.7456880733944953, 2.3109911974054915)</t>
+        </is>
+      </c>
+      <c r="L56" s="1" t="inlineStr">
+        <is>
+          <t>4.952326571837386</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n"/>
-      <c r="F57" s="3" t="n"/>
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>e56</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>e56_24019-32_4_4.jpeg</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>IMG_3076HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F57" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>0.13511054063911565</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>(906, 2.0941367306634957, 1.2117431192660548, 0.7456880733944953, 2.374714266210355)</t>
+        </is>
+      </c>
+      <c r="L57" s="1" t="inlineStr">
+        <is>
+          <t>5.664766534803467</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n"/>
-      <c r="F58" s="3" t="n"/>
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>e57</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>e57_24019-32_4_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>IMG_3076HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F58" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>0.13512246443902026</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>(912, 2.0760443583670276, 1.2117431192660548, 0.7456880733944953, 2.319642371570864)</t>
+        </is>
+      </c>
+      <c r="L58" s="1" t="inlineStr">
+        <is>
+          <t>5.708207995959935</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n"/>
-      <c r="F59" s="3" t="n"/>
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>e58</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>e58_24019-32_4_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>IMG_3076VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F59" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>0.13508977919928172</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>(909, 2.084852257669864, 1.2117431192660548, 0.7456880733944953, 2.33214643037568)</t>
+        </is>
+      </c>
+      <c r="L59" s="1" t="inlineStr">
+        <is>
+          <t>5.76902604157899</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n"/>
-      <c r="F60" s="3" t="n"/>
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>e59</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>e59_24019-32_4_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>IMG_3077.jpeg</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F60" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:35:02</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>0.10927837537739078</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>(1235, 1.5671695066533062, 0.8823821339950371, 0.5357320099255583, 1.746869907970614)</t>
+        </is>
+      </c>
+      <c r="L60" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n"/>
-      <c r="F61" s="3" t="n"/>
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>e60</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>e60_24019-32_4_0.jpeg</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>IMG_3077HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F61" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>0.10935104427710284</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>(1238, 1.5646672370864942, 0.8823821339950371, 0.5357320099255583, 1.7409378576750822)</t>
+        </is>
+      </c>
+      <c r="L61" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n"/>
-      <c r="F62" s="3" t="n"/>
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>e61</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>e61_24019-32_5_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>IMG_3077HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F62" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>0.10937169686819487</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>(1237, 1.5664532857592701, 0.8823821339950371, 0.5357320099255583, 1.7536458069139889)</t>
+        </is>
+      </c>
+      <c r="L62" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n"/>
-      <c r="F63" s="3" t="n"/>
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>e62</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>e62_24019-32_5_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>IMG_3077VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>United Stone International</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Salon, Ohio</t>
+        </is>
+      </c>
+      <c r="F63" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>0.10921147894102745</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>(1233, 1.5711551531680115, 0.8823821339950371, 0.5357320099255583, 1.7536458069139889)</t>
+        </is>
+      </c>
+      <c r="L63" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n"/>
       <c r="F64" s="3" t="n"/>
+      <c r="L64" s="1" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
       <c r="F65" s="3" t="n"/>
+      <c r="L65" s="1" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
       <c r="F66" s="3" t="n"/>
+      <c r="L66" s="1" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
       <c r="F67" s="3" t="n"/>
+      <c r="L67" s="1" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n"/>
       <c r="F68" s="3" t="n"/>
+      <c r="L68" s="1" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
       <c r="F69" s="3" t="n"/>
+      <c r="L69" s="1" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
       <c r="F70" s="3" t="n"/>
+      <c r="L70" s="1" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n"/>
       <c r="F71" s="3" t="n"/>
+      <c r="L71" s="1" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n"/>
       <c r="F72" s="3" t="n"/>
+      <c r="L72" s="1" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
       <c r="F73" s="3" t="n"/>
+      <c r="L73" s="1" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n"/>
       <c r="F74" s="3" t="n"/>
+      <c r="L74" s="1" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n"/>
       <c r="F75" s="3" t="n"/>
+      <c r="L75" s="1" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n"/>
       <c r="F76" s="3" t="n"/>
+      <c r="L76" s="1" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n"/>
       <c r="F77" s="3" t="n"/>
+      <c r="L77" s="1" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
       <c r="F78" s="3" t="n"/>
+      <c r="L78" s="1" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n"/>
       <c r="F79" s="3" t="n"/>
+      <c r="L79" s="1" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n"/>
       <c r="F80" s="3" t="n"/>
+      <c r="L80" s="1" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n"/>
       <c r="F81" s="3" t="n"/>
+      <c r="L81" s="1" t="n"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
       <c r="F82" s="3" t="n"/>
+      <c r="L82" s="1" t="n"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n"/>
       <c r="F83" s="3" t="n"/>
+      <c r="L83" s="1" t="n"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n"/>
       <c r="F84" s="3" t="n"/>
+      <c r="L84" s="1" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
       <c r="F85" s="3" t="n"/>
+      <c r="L85" s="1" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n"/>
       <c r="F86" s="3" t="n"/>
+      <c r="L86" s="1" t="n"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
       <c r="F87" s="3" t="n"/>
+      <c r="L87" s="1" t="n"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n"/>
       <c r="F88" s="3" t="n"/>
+      <c r="L88" s="1" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
       <c r="F89" s="3" t="n"/>
+      <c r="L89" s="1" t="n"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
       <c r="F90" s="3" t="n"/>
+      <c r="L90" s="1" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n"/>
       <c r="F91" s="3" t="n"/>
+      <c r="L91" s="1" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n"/>
       <c r="F92" s="3" t="n"/>
+      <c r="L92" s="1" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n"/>
       <c r="F93" s="3" t="n"/>
+      <c r="L93" s="1" t="n"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
       <c r="F94" s="3" t="n"/>
+      <c r="L94" s="1" t="n"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
       <c r="F95" s="3" t="n"/>
+      <c r="L95" s="1" t="n"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
       <c r="F96" s="3" t="n"/>
+      <c r="L96" s="1" t="n"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n"/>
       <c r="F97" s="3" t="n"/>
+      <c r="L97" s="1" t="n"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n"/>
       <c r="F98" s="3" t="n"/>
+      <c r="L98" s="1" t="n"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n"/>
       <c r="F99" s="3" t="n"/>
+      <c r="L99" s="1" t="n"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n"/>
       <c r="F100" s="3" t="n"/>
+      <c r="L100" s="1" t="n"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n"/>
       <c r="F101" s="3" t="n"/>
+      <c r="L101" s="1" t="n"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n"/>
       <c r="F102" s="3" t="n"/>
+      <c r="L102" s="1" t="n"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n"/>
       <c r="F103" s="3" t="n"/>
+      <c r="L103" s="1" t="n"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n"/>
       <c r="F104" s="3" t="n"/>
+      <c r="L104" s="1" t="n"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n"/>
       <c r="F105" s="3" t="n"/>
+      <c r="L105" s="1" t="n"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n"/>
       <c r="F106" s="3" t="n"/>
+      <c r="L106" s="1" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n"/>
       <c r="F107" s="3" t="n"/>
+      <c r="L107" s="1" t="n"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n"/>
       <c r="F108" s="3" t="n"/>
+      <c r="L108" s="1" t="n"/>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n"/>
       <c r="F109" s="3" t="n"/>
+      <c r="L109" s="1" t="n"/>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n"/>
       <c r="F110" s="3" t="n"/>
+      <c r="L110" s="1" t="n"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n"/>
       <c r="F111" s="3" t="n"/>
+      <c r="L111" s="1" t="n"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n"/>
       <c r="F112" s="3" t="n"/>
+      <c r="L112" s="1" t="n"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n"/>
       <c r="F113" s="3" t="n"/>
+      <c r="L113" s="1" t="n"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n"/>
       <c r="F114" s="3" t="n"/>
+      <c r="L114" s="1" t="n"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n"/>
       <c r="F115" s="3" t="n"/>
+      <c r="L115" s="1" t="n"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n"/>
       <c r="F116" s="3" t="n"/>
+      <c r="L116" s="1" t="n"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n"/>
       <c r="F117" s="3" t="n"/>
+      <c r="L117" s="1" t="n"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n"/>
       <c r="F118" s="3" t="n"/>
+      <c r="L118" s="1" t="n"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n"/>
       <c r="F119" s="3" t="n"/>
+      <c r="L119" s="1" t="n"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n"/>
       <c r="F120" s="3" t="n"/>
+      <c r="L120" s="1" t="n"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n"/>
       <c r="F121" s="3" t="n"/>
+      <c r="L121" s="1" t="n"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n"/>
       <c r="F122" s="3" t="n"/>
+      <c r="L122" s="1" t="n"/>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n"/>
       <c r="F123" s="3" t="n"/>
+      <c r="L123" s="1" t="n"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n"/>
       <c r="F124" s="3" t="n"/>
+      <c r="L124" s="1" t="n"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n"/>
       <c r="F125" s="3" t="n"/>
+      <c r="L125" s="1" t="n"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n"/>
       <c r="F126" s="3" t="n"/>
+      <c r="L126" s="1" t="n"/>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n"/>
       <c r="F127" s="3" t="n"/>
+      <c r="L127" s="1" t="n"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n"/>
       <c r="F128" s="3" t="n"/>
+      <c r="L128" s="1" t="n"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n"/>
       <c r="F129" s="3" t="n"/>
+      <c r="L129" s="1" t="n"/>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n"/>
       <c r="F130" s="3" t="n"/>
+      <c r="L130" s="1" t="n"/>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n"/>
       <c r="F131" s="3" t="n"/>
+      <c r="L131" s="1" t="n"/>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n"/>
       <c r="F132" s="3" t="n"/>
+      <c r="L132" s="1" t="n"/>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n"/>
       <c r="F133" s="3" t="n"/>
+      <c r="L133" s="1" t="n"/>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n"/>
+      <c r="L134" s="1" t="n"/>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n"/>
+      <c r="L135" s="1" t="n"/>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n"/>
+      <c r="L136" s="1" t="n"/>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n"/>
+      <c r="L137" s="1" t="n"/>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n"/>
+      <c r="L138" s="1" t="n"/>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n"/>
+      <c r="L139" s="1" t="n"/>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n"/>
+      <c r="L140" s="1" t="n"/>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n"/>
+      <c r="L141" s="1" t="n"/>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n"/>
+      <c r="L142" s="1" t="n"/>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n"/>
+      <c r="L143" s="1" t="n"/>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n"/>
+      <c r="L144" s="1" t="n"/>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n"/>
+      <c r="L145" s="1" t="n"/>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n"/>
+      <c r="L146" s="1" t="n"/>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n"/>
+      <c r="L147" s="1" t="n"/>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n"/>
+      <c r="L148" s="1" t="n"/>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n"/>
+      <c r="L149" s="1" t="n"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n"/>
+      <c r="L150" s="1" t="n"/>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n"/>
+      <c r="L151" s="1" t="n"/>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n"/>
+      <c r="L152" s="1" t="n"/>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n"/>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-13, last lines (exp, sim, neg): (154, 170, 65)
</commit_message>
<xml_diff>
--- a/manifests/Experiment_Manifest.xlsx
+++ b/manifests/Experiment_Manifest.xlsx
@@ -398,8 +398,8 @@
   </sheetPr>
   <dimension ref="A1:M10001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="46" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:M97"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="46" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:M153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -5524,7 +5524,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5654,7 +5653,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5717,7 +5715,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H84" t="inlineStr"/>
       <c r="I84" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5780,7 +5777,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H85" t="inlineStr"/>
       <c r="I85" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5910,7 +5906,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5973,7 +5968,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6036,7 +6030,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H89" t="inlineStr"/>
       <c r="I89" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6166,7 +6159,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6229,7 +6221,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H92" t="inlineStr"/>
       <c r="I92" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6292,7 +6283,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6422,7 +6412,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H95" t="inlineStr"/>
       <c r="I95" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6485,7 +6474,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6548,7 +6536,6 @@
           <t>24019-32</t>
         </is>
       </c>
-      <c r="H97" t="inlineStr"/>
       <c r="I97" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6576,263 +6563,3567 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="n"/>
-      <c r="F98" s="3" t="n"/>
-      <c r="L98" s="1" t="n"/>
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>e97</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>e97_24019-32_1_1jpeg</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>IMG_3174.jpeg</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F98" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:50</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>0.035976819755617236</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>(549, 1.2210813360751183, 0.622372159090909, 0.3788352272727272, 1.270241107212891)</t>
+        </is>
+      </c>
+      <c r="L98" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="n"/>
-      <c r="F99" s="3" t="n"/>
-      <c r="L99" s="1" t="n"/>
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>e98</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>e98_24019-32_1_2jpeg</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>IMG_3174HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F99" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>0.03601408398841037</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>(557, 1.2034423034908583, 0.622372159090909, 0.3788352272727272, 1.2151003117776003)</t>
+        </is>
+      </c>
+      <c r="L99" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="n"/>
-      <c r="F100" s="3" t="n"/>
-      <c r="L100" s="1" t="n"/>
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>e99</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>e99_24019-32_1_3jpeg</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>IMG_3174HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F100" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>0.03598514273146951</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>(556, 1.2118453452616824, 0.620386921669759, 0.3788352272727272, 1.2362805279500524)</t>
+        </is>
+      </c>
+      <c r="L100" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="n"/>
-      <c r="F101" s="3" t="n"/>
-      <c r="L101" s="1" t="n"/>
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>e100</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>e100_24019-32_1_4jpeg</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>IMG_3174VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F101" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>0.03597970442338422</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>(556, 1.2112043644478063, 0.622372159090909, 0.3788352272727272, 1.2265241846063397)</t>
+        </is>
+      </c>
+      <c r="L101" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="n"/>
-      <c r="F102" s="3" t="n"/>
-      <c r="L102" s="1" t="n"/>
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>e101</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>e101_24019-32_1_5jpeg</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>IMG_3175.jpeg</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F102" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:28:55</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>0.02565776774681468</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>(429, 1.193344491958591, 0.651418592666259, 0.44270152505446614, 1.308798718734383)</t>
+        </is>
+      </c>
+      <c r="L102" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="n"/>
-      <c r="F103" s="3" t="n"/>
-      <c r="L103" s="1" t="n"/>
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>e102</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>e102_24019-32_1_6jpeg</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>IMG_3175HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F103" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>0.025394039646036728</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>(426, 1.2006815483660267, 0.6640522875816992, 0.44270152505446614, 1.313706941723645)</t>
+        </is>
+      </c>
+      <c r="L103" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="n"/>
-      <c r="F104" s="3" t="n"/>
-      <c r="L104" s="1" t="n"/>
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>e103</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>e103_24019-32_1_7jpeg</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>IMG_3175HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F104" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>0.025684071336918517</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>(426, 1.1983660129070648, 0.658482735849933, 0.4169990440320076, 1.345944428094168)</t>
+        </is>
+      </c>
+      <c r="L104" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="n"/>
-      <c r="F105" s="3" t="n"/>
-      <c r="L105" s="1" t="n"/>
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>e104</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>e104_24019-32_1_8jpeg</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>IMG_3175VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F105" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>0.025661179302674014</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>(429, 1.194463632387686, 0.6640522875816992, 0.415032679738562, 1.3180346695693466)</t>
+        </is>
+      </c>
+      <c r="L105" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="n"/>
-      <c r="F106" s="3" t="n"/>
-      <c r="L106" s="1" t="n"/>
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>e105</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>e105_24019-32_2_7jpeg</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>IMG_3176.jpeg</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F106" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:05</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>0.0282690393808343</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>(403, 1.3107682779511318, 0.7368911174785099, 0.46396848137535807, 1.3629160591213492)</t>
+        </is>
+      </c>
+      <c r="L106" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="n"/>
-      <c r="F107" s="3" t="n"/>
-      <c r="L107" s="1" t="n"/>
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>e106</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>e106_24019-32_2_6jpeg</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>IMG_3176HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F107" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>0.02837290052011066</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>(406, 1.3062528016550026, 0.7194086263964772, 0.44166235732935555, 1.3709102149771604)</t>
+        </is>
+      </c>
+      <c r="L107" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="n"/>
-      <c r="F108" s="3" t="n"/>
-      <c r="L108" s="1" t="n"/>
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>e107</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>e107_24019-32_2_5jpeg</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>IMG_3176HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F108" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>0.028284673873777706</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>(411, 1.2941792768850942, 0.7210545726884368, 0.45292170789506925, 1.3747710729450187)</t>
+        </is>
+      </c>
+      <c r="L108" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="n"/>
-      <c r="F109" s="3" t="n"/>
-      <c r="L109" s="1" t="n"/>
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>e108</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>e108_24019-32_2_4jpeg</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>IMG_3176VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F109" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>0.02827875681952528</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>(411, 1.2936517189204129, 0.7141164074561062, 0.449920644955938, 1.373645483931949)</t>
+        </is>
+      </c>
+      <c r="L109" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="n"/>
-      <c r="F110" s="3" t="n"/>
-      <c r="L110" s="1" t="n"/>
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>e109</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>e109_24019-32_2_3jpeg</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>IMG_3177.jpeg</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F110" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:29</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>0.02781007874702744</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>(423, 1.222482883537956, 0.6884712685218648, 0.44062161185399346, 1.3181962857180773)</t>
+        </is>
+      </c>
+      <c r="L110" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="n"/>
-      <c r="F111" s="3" t="n"/>
-      <c r="L111" s="1" t="n"/>
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>e110</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>e110_24019-32_2_2jpeg</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>IMG_3177HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F111" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>0.027876102900504404</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>(431, 1.2052792202714877, 0.6884712685218648, 0.44062161185399346, 1.2898082797822203)</t>
+        </is>
+      </c>
+      <c r="L111" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="n"/>
-      <c r="F112" s="3" t="n"/>
-      <c r="L112" s="1" t="n"/>
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>e111</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>e111_24019-32_2_1jpeg</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>IMG_3177HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F112" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>0.02787649473524314</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>(422, 1.228568973655914, 0.6907582591933163, 0.44062161185399346, 1.321336896284785)</t>
+        </is>
+      </c>
+      <c r="L112" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="n"/>
-      <c r="F113" s="3" t="n"/>
-      <c r="L113" s="1" t="n"/>
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>e112</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>e112_24019-32_2_0jpeg</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>IMG_3177VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F113" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>0.027881343690134994</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>(425, 1.2178382287955398, 0.6815190521645917, 0.44062161185399346, 1.2912806737959508)</t>
+        </is>
+      </c>
+      <c r="L113" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="n"/>
-      <c r="F114" s="3" t="n"/>
-      <c r="L114" s="1" t="n"/>
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>e113</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>e113_24019-32_3_1jpeg</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>IMG_3178.jpeg</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F114" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:35</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>0.022924369605732336</t>
+        </is>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>(461, 1.1696272194592219, 0.6636122680802725, 0.4327906096175691, 1.2489258492171604)</t>
+        </is>
+      </c>
+      <c r="L114" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="n"/>
-      <c r="F115" s="3" t="n"/>
-      <c r="L115" s="1" t="n"/>
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>e114</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>e114_24019-32_3_2jpeg</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>IMG_3178HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F115" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>0.022951144256081208</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>(460, 1.17172470237719, 0.6598344953300344, 0.4327906096175691, 1.2442618019573477)</t>
+        </is>
+      </c>
+      <c r="L115" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="n"/>
-      <c r="F116" s="3" t="n"/>
-      <c r="L116" s="1" t="n"/>
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>e115</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>e115_24019-32_3_3jpeg</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>IMG_3178HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F116" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>0.02298512333041954</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>(466, 1.1607730163946821, 0.6347595607724347, 0.4044505270034219, 1.2392886214067258)</t>
+        </is>
+      </c>
+      <c r="L116" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="n"/>
-      <c r="F117" s="3" t="n"/>
-      <c r="L117" s="1" t="n"/>
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>e116</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>e116_24019-32_3_4jpeg</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>IMG_3178VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F117" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>0.02291517590049206</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>(462, 1.1679289713086738, 0.6399628547623702, 0.461643316925407, 1.246042901247536)</t>
+        </is>
+      </c>
+      <c r="L117" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="n"/>
-      <c r="F118" s="3" t="n"/>
-      <c r="L118" s="1" t="n"/>
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>e117</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>e117_24019-32_3_5jpeg</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>IMG_3179.jpeg</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F118" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:46</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>0.02794206571402925</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>(435, 1.2582953417980787, 0.7048250405697503, 0.4069474744182705, 1.3658435464062773)</t>
+        </is>
+      </c>
+      <c r="L118" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="n"/>
-      <c r="F119" s="3" t="n"/>
-      <c r="L119" s="1" t="n"/>
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>e118</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>e118_24019-32_3_6jpeg</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>IMG_3179HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F119" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>0.027880598655863054</t>
+        </is>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>(434, 1.261013295913934, 0.6870335786355479, 0.42138551292729076, 1.3927012515556347)</t>
+        </is>
+      </c>
+      <c r="L119" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="n"/>
-      <c r="F120" s="3" t="n"/>
-      <c r="L120" s="1" t="n"/>
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t>e119</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>e119_24019-32_3_7jpeg</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>IMG_3179HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F120" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>0.027892838384476062</t>
+        </is>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>(438, 1.255288969731367, 0.67023202554863, 0.4169702716525152, 1.390751649841509)</t>
+        </is>
+      </c>
+      <c r="L120" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="n"/>
-      <c r="F121" s="3" t="n"/>
-      <c r="L121" s="1" t="n"/>
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>e120</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>e120_24019-32_3_8jpeg</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>IMG_3179VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F121" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>0.027949688702902264</t>
+        </is>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>(439, 1.2525909080286008, 0.7106554032611887, 0.45301985167819075, 1.3746879895680673)</t>
+        </is>
+      </c>
+      <c r="L121" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="n"/>
-      <c r="F122" s="3" t="n"/>
-      <c r="L122" s="1" t="n"/>
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>e121</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>e121_24019-32_4_7jpeg</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>IMG_3180.jpeg</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F122" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>2020-07-09 15:29:53</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>0.02224532398965588</t>
+        </is>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>(404, 1.2033132445352663, 0.6295155839279007, 0.4578295155839278, 1.213278623217117)</t>
+        </is>
+      </c>
+      <c r="L122" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="n"/>
-      <c r="F123" s="3" t="n"/>
-      <c r="L123" s="1" t="n"/>
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>e122</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>e122_24019-32_4_6jpeg</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>IMG_3180HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F123" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>0.022329138304936463</t>
+        </is>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>(405, 1.2056513581677402, 0.6295155839279007, 0.4578295155839278, 1.2412141443786293)</t>
+        </is>
+      </c>
+      <c r="L123" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="n"/>
-      <c r="F124" s="3" t="n"/>
-      <c r="L124" s="1" t="n"/>
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>e123</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>e123_24019-32_4_5jpeg</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>IMG_3180HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F124" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>0.022353515843954976</t>
+        </is>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>(404, 1.2076887508330563, 0.6295155839279007, 0.4578295155839278, 1.238556539327241)</t>
+        </is>
+      </c>
+      <c r="L124" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="n"/>
-      <c r="F125" s="3" t="n"/>
-      <c r="L125" s="1" t="n"/>
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t>e124</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>e124_24019-32_4_4jpeg</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>IMG_3180VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F125" s="3" t="inlineStr">
+        <is>
+          <t>Dallas White</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>0.022329032545548095</t>
+        </is>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>(399, 1.2079370810407037, 0.6295155839279007, 0.4578295155839278, 1.208907754935909)</t>
+        </is>
+      </c>
+      <c r="L125" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="n"/>
-      <c r="F126" s="3" t="n"/>
-      <c r="L126" s="1" t="n"/>
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t>e125</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>e125_24019-32_1_1jpeg</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>IMG_3070.jpeg</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F126" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:33:40</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>0.10626314137255605</t>
+        </is>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>(1766, 1.2229455581121895, 0.6614104882459312, 0.413381555153707, 1.2921876388374214)</t>
+        </is>
+      </c>
+      <c r="L126" s="1" t="inlineStr">
+        <is>
+          <t>165.27474785372564</t>
+        </is>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="n"/>
-      <c r="F127" s="3" t="n"/>
-      <c r="L127" s="1" t="n"/>
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>e126</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>e126_24019-32_1_2jpeg</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>IMG_3070HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F127" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>0.10629850658417507</t>
+        </is>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>(1766, 1.2199003546381992, 0.6614104882459312, 0.413381555153707, 1.2678898364915758)</t>
+        </is>
+      </c>
+      <c r="L127" s="1" t="inlineStr">
+        <is>
+          <t>176.2933681716365</t>
+        </is>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="n"/>
-      <c r="F128" s="3" t="n"/>
-      <c r="L128" s="1" t="n"/>
+      <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t>e127</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>e127_24019-32_1_3jpeg</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>IMG_3070HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F128" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr"/>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>0.10635143177604318</t>
+        </is>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>(1762, 1.225678035511058, 0.6614104882459312, 0.413381555153707, 1.2904231659976855)</t>
+        </is>
+      </c>
+      <c r="L128" s="1" t="inlineStr">
+        <is>
+          <t>171.15013017929488</t>
+        </is>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="n"/>
-      <c r="F129" s="3" t="n"/>
-      <c r="L129" s="1" t="n"/>
+      <c r="A129" s="1" t="inlineStr">
+        <is>
+          <t>e128</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>e128_24019-32_1_4jpeg</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>IMG_3070VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F129" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>0.10632121683796092</t>
+        </is>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>(1765, 1.2229526718381063, 0.6614104882459312, 0.413381555153707, 1.2822941522156464)</t>
+        </is>
+      </c>
+      <c r="L129" s="1" t="inlineStr">
+        <is>
+          <t>172.45188887966015</t>
+        </is>
+      </c>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="n"/>
-      <c r="F130" s="3" t="n"/>
-      <c r="L130" s="1" t="n"/>
+      <c r="A130" s="1" t="inlineStr">
+        <is>
+          <t>e129</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>e129_24019-32_1_5jpeg</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>IMG_3071.jpeg</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F130" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:33:48</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>0.08643496713420627</t>
+        </is>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>(1684, 1.2069945549279888, 0.708973149761974, 0.4385611510791366, 1.3806035251687194)</t>
+        </is>
+      </c>
+      <c r="L130" s="1" t="inlineStr">
+        <is>
+          <t>94.42038980384035</t>
+        </is>
+      </c>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="131">
-      <c r="A131" s="1" t="n"/>
-      <c r="F131" s="3" t="n"/>
-      <c r="L131" s="1" t="n"/>
+      <c r="A131" s="1" t="inlineStr">
+        <is>
+          <t>e130</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>e130_24019-32_1_6jpeg</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>IMG_3071HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F131" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr"/>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>0.08652764479064227</t>
+        </is>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>(1694, 1.2008022668874019, 0.6863044771772961, 0.4385611510791366, 1.3775864387972148)</t>
+        </is>
+      </c>
+      <c r="L131" s="1" t="inlineStr">
+        <is>
+          <t>100.28212637027066</t>
+        </is>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="n"/>
-      <c r="F132" s="3" t="n"/>
-      <c r="L132" s="1" t="n"/>
+      <c r="A132" s="1" t="inlineStr">
+        <is>
+          <t>e131</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>e131_24019-32_1_7jpeg</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>IMG_3071HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F132" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr"/>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>0.08649615379638731</t>
+        </is>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>(1690, 1.2043601987317867, 0.6989554419433464, 0.4385611510791366, 1.3803898557031795)</t>
+        </is>
+      </c>
+      <c r="L132" s="1" t="inlineStr">
+        <is>
+          <t>98.4263856218622</t>
+        </is>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="133">
-      <c r="A133" s="1" t="n"/>
-      <c r="F133" s="3" t="n"/>
-      <c r="L133" s="1" t="n"/>
+      <c r="A133" s="1" t="inlineStr">
+        <is>
+          <t>e132</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>e132_24019-32_1_8jpeg</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>IMG_3071VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F133" s="3" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr"/>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>0.08645835489881472</t>
+        </is>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>(1696, 1.199935426463319, 0.6956412016185844, 0.4385611510791366, 1.366295785404334)</t>
+        </is>
+      </c>
+      <c r="L133" s="1" t="inlineStr">
+        <is>
+          <t>98.1003161948139</t>
+        </is>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="134">
-      <c r="A134" s="1" t="n"/>
-      <c r="L134" s="1" t="n"/>
+      <c r="A134" s="1" t="inlineStr">
+        <is>
+          <t>e133</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>e133_24019-32_2_7jpeg</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>IMG_3072.jpeg</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:33:56</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>0.13068273945587136</t>
+        </is>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>(1502, 1.3665101504291362, 0.6695283064779868, 0.4430232558139534, 1.358199999090961)</t>
+        </is>
+      </c>
+      <c r="L134" s="1" t="inlineStr">
+        <is>
+          <t>143.29521206564354</t>
+        </is>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="135">
-      <c r="A135" s="1" t="n"/>
-      <c r="L135" s="1" t="n"/>
+      <c r="A135" s="1" t="inlineStr">
+        <is>
+          <t>e134</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>e134_24019-32_2_6jpeg</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>IMG_3072HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr"/>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>0.13067947148374115</t>
+        </is>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>(1496, 1.3698571109802948, 0.6695283064779868, 0.4430232558139534, 1.3584396791263003)</t>
+        </is>
+      </c>
+      <c r="L135" s="1" t="inlineStr">
+        <is>
+          <t>145.40357696516693</t>
+        </is>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="136">
-      <c r="A136" s="1" t="n"/>
-      <c r="L136" s="1" t="n"/>
+      <c r="A136" s="1" t="inlineStr">
+        <is>
+          <t>e135</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>e135_24019-32_2_5jpeg</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>IMG_3072HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr"/>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>0.13067630254106943</t>
+        </is>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>(1494, 1.3735578691894301, 0.6767066767292842, 0.4430232558139534, 1.3801462356689742)</t>
+        </is>
+      </c>
+      <c r="L136" s="1" t="inlineStr">
+        <is>
+          <t>145.38977675855187</t>
+        </is>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="137">
-      <c r="A137" s="1" t="n"/>
-      <c r="L137" s="1" t="n"/>
+      <c r="A137" s="1" t="inlineStr">
+        <is>
+          <t>e136</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>e136_24019-32_2_4jpeg</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>IMG_3072VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr"/>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>0.1306894239443195</t>
+        </is>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>(1496, 1.3723766916619047, 0.6735267681936303, 0.4430232558139534, 1.3741309807445359)</t>
+        </is>
+      </c>
+      <c r="L137" s="1" t="inlineStr">
+        <is>
+          <t>145.88505084040355</t>
+        </is>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="138">
-      <c r="A138" s="1" t="n"/>
-      <c r="L138" s="1" t="n"/>
+      <c r="A138" s="1" t="inlineStr">
+        <is>
+          <t>e137</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>e137_24019-32_2_3jpeg</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>IMG_3073.jpeg</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:34:06</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>0.10439114517834187</t>
+        </is>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>(1211, 1.5302384468465018, 0.8603792236850193, 0.5311338289962824, 1.7103870535757584)</t>
+        </is>
+      </c>
+      <c r="L138" s="1" t="inlineStr">
+        <is>
+          <t>5.845177149984105</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="139">
-      <c r="A139" s="1" t="n"/>
-      <c r="L139" s="1" t="n"/>
+      <c r="A139" s="1" t="inlineStr">
+        <is>
+          <t>e138</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>e138_24019-32_2_2jpeg</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>IMG_3073HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr"/>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>0.104415518416343</t>
+        </is>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>(1214, 1.529431913959941, 0.8610819429311831, 0.5311338289962824, 1.7238646636287058)</t>
+        </is>
+      </c>
+      <c r="L139" s="1" t="inlineStr">
+        <is>
+          <t>5.988109409764926</t>
+        </is>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="140">
-      <c r="A140" s="1" t="n"/>
-      <c r="L140" s="1" t="n"/>
+      <c r="A140" s="1" t="inlineStr">
+        <is>
+          <t>e139</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>e139_24019-32_2_1jpeg</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>IMG_3073HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr"/>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>0.10442685480611097</t>
+        </is>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>(1218, 1.5254308696049177, 0.8315038816623117, 0.5311338289962824, 1.709941190842706)</t>
+        </is>
+      </c>
+      <c r="L140" s="1" t="inlineStr">
+        <is>
+          <t>6.253913261287154</t>
+        </is>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="141">
-      <c r="A141" s="1" t="n"/>
-      <c r="L141" s="1" t="n"/>
+      <c r="A141" s="1" t="inlineStr">
+        <is>
+          <t>e140</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>e140_24019-32_2_0jpeg</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>IMG_3073VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr"/>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>0.10446936626774085</t>
+        </is>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>(1218, 1.525646741059214, 0.8514802573194831, 0.5311338289962824, 1.7173242797459052)</t>
+        </is>
+      </c>
+      <c r="L141" s="1" t="inlineStr">
+        <is>
+          <t>6.268958762316714</t>
+        </is>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="142">
-      <c r="A142" s="1" t="n"/>
-      <c r="L142" s="1" t="n"/>
+      <c r="A142" s="1" t="inlineStr">
+        <is>
+          <t>e141</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>e141_24019-32_3_1jpeg</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>IMG_3074.jpeg</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:34:22</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>0.11056792245481</t>
+        </is>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>(1088, 1.676076645824256, 0.913030454318522, 0.5885471491007104, 1.8759228734454052)</t>
+        </is>
+      </c>
+      <c r="L142" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="143">
-      <c r="A143" s="1" t="n"/>
-      <c r="L143" s="1" t="n"/>
+      <c r="A143" s="1" t="inlineStr">
+        <is>
+          <t>e142</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>e142_24019-32_3_2jpeg</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>IMG_3074HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr"/>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>0.11065494244903235</t>
+        </is>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>(1091, 1.6715908328300884, 0.913030454318522, 0.6014683101867633, 1.8816739199934616)</t>
+        </is>
+      </c>
+      <c r="L143" s="1" t="inlineStr">
+        <is>
+          <t>3.143459468809765</t>
+        </is>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="144">
-      <c r="A144" s="1" t="n"/>
-      <c r="L144" s="1" t="n"/>
+      <c r="A144" s="1" t="inlineStr">
+        <is>
+          <t>e143</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>e143_24019-32_3_3jpeg</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>IMG_3074HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr"/>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>0.11066092448945149</t>
+        </is>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>(1087, 1.678747266795845, 0.913030454318522, 0.5813002364269473, 1.8866639498871733)</t>
+        </is>
+      </c>
+      <c r="L144" s="1" t="inlineStr">
+        <is>
+          <t>4.914911766150074</t>
+        </is>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="n"/>
-      <c r="L145" s="1" t="n"/>
+      <c r="A145" s="1" t="inlineStr">
+        <is>
+          <t>e144</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>e144_24019-32_3_4jpeg</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>IMG_3074VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr"/>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>0.11057754980110956</t>
+        </is>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>(1081, 1.68491820145904, 0.913030454318522, 0.5946935894189962, 1.9057548714019261)</t>
+        </is>
+      </c>
+      <c r="L145" s="1" t="inlineStr">
+        <is>
+          <t>3.1203032296288455</t>
+        </is>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="146">
-      <c r="A146" s="1" t="n"/>
-      <c r="L146" s="1" t="n"/>
+      <c r="A146" s="1" t="inlineStr">
+        <is>
+          <t>e145</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>e145_24019-32_3_5jpeg</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>IMG_3075.jpeg</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:34:29</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>0.08209072082885052</t>
+        </is>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>(1118, 1.4621469360083703, 0.9200331451356919, 0.608079800498753, 1.7115512495008964)</t>
+        </is>
+      </c>
+      <c r="L146" s="1" t="inlineStr">
+        <is>
+          <t>6.860800616911583</t>
+        </is>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="147">
-      <c r="A147" s="1" t="n"/>
-      <c r="L147" s="1" t="n"/>
+      <c r="A147" s="1" t="inlineStr">
+        <is>
+          <t>e146</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>e146_24019-32_3_6jpeg</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>IMG_3075HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr"/>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>0.08200434076902503</t>
+        </is>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>(1126, 1.4496896359848837, 0.903816929338094, 0.572775744271396, 1.6973093081113473)</t>
+        </is>
+      </c>
+      <c r="L147" s="1" t="inlineStr">
+        <is>
+          <t>9.08514439586818</t>
+        </is>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="148">
-      <c r="A148" s="1" t="n"/>
-      <c r="L148" s="1" t="n"/>
+      <c r="A148" s="1" t="inlineStr">
+        <is>
+          <t>e147</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>e147_24019-32_3_7jpeg</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>IMG_3075HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr"/>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>0.0820862432447559</t>
+        </is>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>(1121, 1.4589576859822246, 0.917424833211809, 0.6008683417975496, 1.6987361241863967)</t>
+        </is>
+      </c>
+      <c r="L148" s="1" t="inlineStr">
+        <is>
+          <t>7.767870677421157</t>
+        </is>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="149">
-      <c r="A149" s="1" t="n"/>
-      <c r="L149" s="1" t="n"/>
+      <c r="A149" s="1" t="inlineStr">
+        <is>
+          <t>e148</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>e148_24019-32_3_8jpeg</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>IMG_3075VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr"/>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>0.08209650437497275</t>
+        </is>
+      </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>(1117, 1.4629038457113364, 0.9376825215863195, 0.608079800498753, 1.7104042501193422)</t>
+        </is>
+      </c>
+      <c r="L149" s="1" t="inlineStr">
+        <is>
+          <t>6.387044279575373</t>
+        </is>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="150">
-      <c r="A150" s="1" t="n"/>
-      <c r="L150" s="1" t="n"/>
+      <c r="A150" s="1" t="inlineStr">
+        <is>
+          <t>e149</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>e149_24019-32_4_7jpeg</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>IMG_3076.jpeg</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:34:40</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>0.13693333894453324</t>
+        </is>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>(909, 2.084359830935198, 1.2117431192660548, 0.7456880733944953, 2.3109911974054915)</t>
+        </is>
+      </c>
+      <c r="L150" s="1" t="inlineStr">
+        <is>
+          <t>4.952326571837386</t>
+        </is>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="151">
-      <c r="A151" s="1" t="n"/>
-      <c r="L151" s="1" t="n"/>
+      <c r="A151" s="1" t="inlineStr">
+        <is>
+          <t>e150</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>e150_24019-32_4_6jpeg</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>IMG_3076HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr"/>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>0.13511054063911565</t>
+        </is>
+      </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>(906, 2.0941367306634957, 1.2117431192660548, 0.7456880733944953, 2.374714266210355)</t>
+        </is>
+      </c>
+      <c r="L151" s="1" t="inlineStr">
+        <is>
+          <t>5.664766534803467</t>
+        </is>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="152">
-      <c r="A152" s="1" t="n"/>
-      <c r="L152" s="1" t="n"/>
+      <c r="A152" s="1" t="inlineStr">
+        <is>
+          <t>e151</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>e151_24019-32_4_5jpeg</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>IMG_3076HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr"/>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>0.13512246443902026</t>
+        </is>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>(912, 2.0760443583670276, 1.2117431192660548, 0.7456880733944953, 2.319642371570864)</t>
+        </is>
+      </c>
+      <c r="L152" s="1" t="inlineStr">
+        <is>
+          <t>5.708207995959935</t>
+        </is>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="153">
-      <c r="A153" s="1" t="n"/>
+      <c r="A153" s="1" t="inlineStr">
+        <is>
+          <t>e152</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>e152_24019-32_4_4jpeg</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>IMG_3076VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>USI</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Solon, OH</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Luna Pearl</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>24019-32</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr"/>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>0.13508977919928172</t>
+        </is>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>(909, 2.084852257669864, 1.2117431192660548, 0.7456880733944953, 2.33214643037568)</t>
+        </is>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>5.76902604157899</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n"/>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-13, last lines (exp, sim, neg): (154, 170, 88)
</commit_message>
<xml_diff>
--- a/manifests/Experiment_Manifest.xlsx
+++ b/manifests/Experiment_Manifest.xlsx
@@ -9370,7 +9370,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>IMG_3074.jpeg</t>
+          <t>IMG_3088.jpeg</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -9395,7 +9395,7 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>2020-07-09 14:34:22</t>
+          <t>2020-07-09 14:37:07</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
@@ -9405,17 +9405,17 @@
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>0.11056792245481</t>
+          <t>0.11535204198487282</t>
         </is>
       </c>
       <c r="K142" t="inlineStr">
         <is>
-          <t>(1088, 1.676076645824256, 0.913030454318522, 0.5885471491007104, 1.8759228734454052)</t>
+          <t>(1484, 1.3251781589586782, 0.6561894510226047, 0.4158902096809156, 1.3509771019612011)</t>
         </is>
       </c>
       <c r="L142" s="1" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>227.33670581119546</t>
         </is>
       </c>
       <c r="M142" t="inlineStr">
@@ -9437,7 +9437,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>IMG_3074HorFlip.jpeg</t>
+          <t>IMG_3088HorFlip.jpeg</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -9468,17 +9468,17 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>0.11065494244903235</t>
+          <t>0.11533485469790346</t>
         </is>
       </c>
       <c r="K143" t="inlineStr">
         <is>
-          <t>(1091, 1.6715908328300884, 0.913030454318522, 0.6014683101867633, 1.8816739199934616)</t>
+          <t>(1493, 1.318581041000772, 0.6561894510226047, 0.4158902096809156, 1.344388817002186)</t>
         </is>
       </c>
       <c r="L143" s="1" t="inlineStr">
         <is>
-          <t>3.143459468809765</t>
+          <t>236.99495750491567</t>
         </is>
       </c>
       <c r="M143" t="inlineStr">
@@ -9500,7 +9500,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>IMG_3074HorVertFlip.jpeg</t>
+          <t>IMG_3088HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -9531,17 +9531,17 @@
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t>0.11066092448945149</t>
+          <t>0.11537656766403137</t>
         </is>
       </c>
       <c r="K144" t="inlineStr">
         <is>
-          <t>(1087, 1.678747266795845, 0.913030454318522, 0.5813002364269473, 1.8866639498871733)</t>
+          <t>(1487, 1.3237520360761383, 0.6535506917915219, 0.4120614880746857, 1.3543781168633076)</t>
         </is>
       </c>
       <c r="L144" s="1" t="inlineStr">
         <is>
-          <t>4.914911766150074</t>
+          <t>231.6619878777485</t>
         </is>
       </c>
       <c r="M144" t="inlineStr">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>IMG_3074VertFlip.jpeg</t>
+          <t>IMG_3088VertFlip.jpeg</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -9594,17 +9594,17 @@
       </c>
       <c r="J145" t="inlineStr">
         <is>
-          <t>0.11057754980110956</t>
+          <t>0.11534055160762927</t>
         </is>
       </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>(1081, 1.68491820145904, 0.913030454318522, 0.5946935894189962, 1.9057548714019261)</t>
+          <t>(1486, 1.3243619875569776, 0.6561894510226047, 0.41060417718551745, 1.3550973083815085)</t>
         </is>
       </c>
       <c r="L145" s="1" t="inlineStr">
         <is>
-          <t>3.1203032296288455</t>
+          <t>238.8518535735845</t>
         </is>
       </c>
       <c r="M145" t="inlineStr">
@@ -9626,7 +9626,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>IMG_3075.jpeg</t>
+          <t>IMG_3089.jpeg</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -9651,7 +9651,7 @@
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>2020-07-09 14:34:29</t>
+          <t>2020-07-09 14:37:19</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
@@ -9661,17 +9661,17 @@
       </c>
       <c r="J146" t="inlineStr">
         <is>
-          <t>0.08209072082885052</t>
+          <t>0.11345984617718798</t>
         </is>
       </c>
       <c r="K146" t="inlineStr">
         <is>
-          <t>(1118, 1.4621469360083703, 0.9200331451356919, 0.608079800498753, 1.7115512495008964)</t>
+          <t>(1480, 1.4087008619651584, 0.7815384615384615, 0.48094674556213013, 1.5422889457155255)</t>
         </is>
       </c>
       <c r="L146" s="1" t="inlineStr">
         <is>
-          <t>6.860800616911583</t>
+          <t>49.57618974125555</t>
         </is>
       </c>
       <c r="M146" t="inlineStr">
@@ -9693,7 +9693,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>IMG_3075HorFlip.jpeg</t>
+          <t>IMG_3089HorFlip.jpeg</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -9724,17 +9724,17 @@
       </c>
       <c r="J147" t="inlineStr">
         <is>
-          <t>0.08200434076902503</t>
+          <t>0.11359627930861428</t>
         </is>
       </c>
       <c r="K147" t="inlineStr">
         <is>
-          <t>(1126, 1.4496896359848837, 0.903816929338094, 0.572775744271396, 1.6973093081113473)</t>
+          <t>(1465, 1.4217420955967701, 0.7815384615384615, 0.48094674556213013, 1.540281771285855)</t>
         </is>
       </c>
       <c r="L147" s="1" t="inlineStr">
         <is>
-          <t>9.08514439586818</t>
+          <t>51.25137848114561</t>
         </is>
       </c>
       <c r="M147" t="inlineStr">
@@ -9756,7 +9756,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>IMG_3075HorVertFlip.jpeg</t>
+          <t>IMG_3089HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -9787,17 +9787,17 @@
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>0.0820862432447559</t>
+          <t>0.11349923555431063</t>
         </is>
       </c>
       <c r="K148" t="inlineStr">
         <is>
-          <t>(1121, 1.4589576859822246, 0.917424833211809, 0.6008683417975496, 1.6987361241863967)</t>
+          <t>(1464, 1.4203985543054936, 0.7815384615384615, 0.48094674556213013, 1.5355231232871733)</t>
         </is>
       </c>
       <c r="L148" s="1" t="inlineStr">
         <is>
-          <t>7.767870677421157</t>
+          <t>50.73454570918384</t>
         </is>
       </c>
       <c r="M148" t="inlineStr">
@@ -9819,7 +9819,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>IMG_3075VertFlip.jpeg</t>
+          <t>IMG_3089VertFlip.jpeg</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -9850,17 +9850,17 @@
       </c>
       <c r="J149" t="inlineStr">
         <is>
-          <t>0.08209650437497275</t>
+          <t>0.11355432232764957</t>
         </is>
       </c>
       <c r="K149" t="inlineStr">
         <is>
-          <t>(1117, 1.4629038457113364, 0.9376825215863195, 0.608079800498753, 1.7104042501193422)</t>
+          <t>(1478, 1.4127880980248309, 0.7832788377951785, 0.48094674556213013, 1.5302820488604372)</t>
         </is>
       </c>
       <c r="L149" s="1" t="inlineStr">
         <is>
-          <t>6.387044279575373</t>
+          <t>50.642383221875974</t>
         </is>
       </c>
       <c r="M149" t="inlineStr">
@@ -9882,7 +9882,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>IMG_3076.jpeg</t>
+          <t>IMG_3091.jpeg</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -9907,7 +9907,7 @@
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>2020-07-09 14:34:40</t>
+          <t>2020-07-09 14:37:40</t>
         </is>
       </c>
       <c r="I150" t="inlineStr">
@@ -9917,17 +9917,17 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>0.13693333894453324</t>
+          <t>0.09004301652403991</t>
         </is>
       </c>
       <c r="K150" t="inlineStr">
         <is>
-          <t>(909, 2.084359830935198, 1.2117431192660548, 0.7456880733944953, 2.3109911974054915)</t>
+          <t>(1545, 1.2423789494067314, 0.7121204239297406, 0.4368326764600501, 1.3942848221108175)</t>
         </is>
       </c>
       <c r="L150" s="1" t="inlineStr">
         <is>
-          <t>4.952326571837386</t>
+          <t>183.56257649061618</t>
         </is>
       </c>
       <c r="M150" t="inlineStr">
@@ -9949,7 +9949,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>IMG_3076HorFlip.jpeg</t>
+          <t>IMG_3091HorFlip.jpeg</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -9980,17 +9980,17 @@
       </c>
       <c r="J151" t="inlineStr">
         <is>
-          <t>0.13511054063911565</t>
+          <t>0.09004763802266097</t>
         </is>
       </c>
       <c r="K151" t="inlineStr">
         <is>
-          <t>(906, 2.0941367306634957, 1.2117431192660548, 0.7456880733944953, 2.374714266210355)</t>
+          <t>(1554, 1.237050341535482, 0.7161899890962575, 0.4368326764600501, 1.3918335075056016)</t>
         </is>
       </c>
       <c r="L151" s="1" t="inlineStr">
         <is>
-          <t>5.664766534803467</t>
+          <t>186.8035822673611</t>
         </is>
       </c>
       <c r="M151" t="inlineStr">
@@ -10012,7 +10012,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>IMG_3076HorVertFlip.jpeg</t>
+          <t>IMG_3091HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -10043,17 +10043,17 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>0.13512246443902026</t>
+          <t>0.09004426817991644</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
         <is>
-          <t>(912, 2.0760443583670276, 1.2117431192660548, 0.7456880733944953, 2.319642371570864)</t>
+          <t>(1546, 1.2430971834978908, 0.7161899890962575, 0.4368326764600501, 1.3924041562164096)</t>
         </is>
       </c>
       <c r="L152" s="1" t="inlineStr">
         <is>
-          <t>5.708207995959935</t>
+          <t>188.28394967136646</t>
         </is>
       </c>
       <c r="M152" t="inlineStr">
@@ -10075,7 +10075,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>IMG_3076VertFlip.jpeg</t>
+          <t>IMG_3091VertFlip.jpeg</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -10106,17 +10106,17 @@
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>0.13508977919928172</t>
+          <t>0.09003863572847202</t>
         </is>
       </c>
       <c r="K153" t="inlineStr">
         <is>
-          <t>(909, 2.084852257669864, 1.2117431192660548, 0.7456880733944953, 2.33214643037568)</t>
+          <t>(1543, 1.243353895490931, 0.7143722714501786, 0.4368326764600501, 1.3950472050345757)</t>
         </is>
       </c>
       <c r="L153" t="inlineStr">
         <is>
-          <t>5.76902604157899</t>
+          <t>191.19101557047065</t>
         </is>
       </c>
       <c r="M153" t="inlineStr">

</xml_diff>